<commit_message>
update the achievement list
</commit_message>
<xml_diff>
--- a/achievementSet_full/2.4_ch.xlsx
+++ b/achievementSet_full/2.4_ch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\githubMaintain\starRailScanner\achievementSet_full\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EEAAA2-7D68-41AF-84E0-0EBDF6345D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8784EE9-E488-4BC9-B4F0-07CF475A1FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{6F58AD7D-36FD-4D08-9DD6-51FD0D6CADE0}"/>
   </bookViews>
@@ -6367,34 +6367,7 @@
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
     <cellStyle name="常规 3" xfId="2" xr:uid="{772C5554-958C-4437-8F8A-46C08413E45B}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF9C99"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF10253F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FF98D7B6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF10253F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -7858,10 +7831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99589015-A4E2-4355-A523-BD9E6D5D36D9}">
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -11461,7 +11434,7 @@
     </row>
     <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A157" s="5">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>75</v>
@@ -11871,12 +11844,6 @@
       </c>
       <c r="G174" s="4" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A175">
-        <f>COUNTIF(A1:A174,2.2)</f>
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -12231,7 +12198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C121D6-321D-41CE-9028-D4F6C58528D9}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>